<commit_message>
new variables, new cleaning of dishes
</commit_message>
<xml_diff>
--- a/Cleaned_Food_Diary.xlsx
+++ b/Cleaned_Food_Diary.xlsx
@@ -477,10 +477,14 @@
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Rice, BR-28, boiled* (without salt) {3.0}; UNKNOWN; Chilli, red, dry {0.1}; Soybean oil {0.15}</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr"/>
+          <t>Rice, BR-28, boiled* (without salt) {3.0}; Small fish fry* {1.5}</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Small fish fry*</t>
+        </is>
+      </c>
       <c r="F2" t="inlineStr">
         <is>
           <t>Rice: Assuming 1 plate = 1 cup cooked rice, or 180 g; Fish filet: Estimate of serving size, and Small Fish fry recipe in food composition table contains other listed ingredients. What to do about salt in dishes, everything is without salt in food composition table?</t>
@@ -503,7 +507,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>UNKNOWN; Onion, raw {1.8}</t>
+          <t>Ruti* {1.0}; Onion, raw {1.8}</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
@@ -525,7 +529,7 @@
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Rice, BR-28, boiled* (without salt) {3.0}; Pangas, without bones, raw {0.97}; Pangas, without bones, raw {0.97}; Potato, Diamond, boiled* (without salt) {0.53}; Brinjal, purple, long, boiled* (without salt) {0.53}</t>
+          <t>Rice, BR-28, boiled* (without salt) {3.0}; Pangas, without bones, raw {0.53}; Pangas, without bones, raw {0.53}; Potato, Diamond, boiled* (without salt) {0.97}; Brinjal, purple, long, boiled* (without salt) {0.97}</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -541,10 +545,22 @@
     </row>
     <row r="5">
       <c r="A5" t="inlineStr"/>
-      <c r="B5" t="inlineStr"/>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>chicken (ootato with bread)</t>
+        </is>
+      </c>
       <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Chicken leg, without skin, raw {1.05}; Potato, Diamond, boiled* (without salt) {0.97}; Bread, bun/roll {0.97}</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Chicken leg, without skin, raw</t>
+        </is>
+      </c>
       <c r="F5" t="inlineStr"/>
     </row>
     <row r="6">
@@ -585,7 +601,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Rice, BR-28, boiled* (without salt) {3.0}; Egg, chicken, farmed, boiled* (without salt) {0.33}; Potato, Diamond, boiled* (without salt) {0.09}; Onion, raw {0.09}; Turmeric, dried {0.1}; Chilli, red, dry {0.1}; Soybean oil {0.15}</t>
+          <t>Rice, BR-28, boiled* (without salt) {3.0}; Egg, chicken, farmed, boiled* (without salt) {0.17}; Potato, Diamond, boiled* (without salt) {0.16}; Onion, raw {0.16}; Turmeric, dried {0.1}; Chilli, red, dry {0.1}; Soybean oil {0.15}</t>
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
@@ -607,7 +623,7 @@
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Rice, BR-28, boiled* (without salt) {3.0}; Egg, chicken, farmed, boiled* (without salt) {1.95}; Potato, Diamond, boiled* (without salt) {0.53}; Onion, raw {0.53}; Turmeric, dried {0.1}; Chilli, red, dry {0.1}; Soybean oil {0.15}</t>
+          <t>Rice, BR-28, boiled* (without salt) {3.0}; Egg, chicken, farmed, boiled* (without salt) {1.05}; Potato, Diamond, boiled* (without salt) {0.97}; Onion, raw {0.97}; Turmeric, dried {0.1}; Chilli, red, dry {0.1}; Soybean oil {0.15}</t>
         </is>
       </c>
       <c r="E8" t="inlineStr"/>
@@ -641,7 +657,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>UNKNOWN; UNKNOWN; UNKNOWN; Papaya, unripe, boiled* (without salt) {0.5}; Green gram, split, boiled* (without salt) {0.5}; Soybean oil {0.15}; Onion, raw {0.5}; Garlic, raw {0.5}</t>
+          <t>UNKNOWN; UNKNOWN; Potato, Diamond, boiled* (without salt) {0.9}; Papaya, unripe, boiled* (without salt) {0.9}; Green gram, split, boiled* (without salt) {0.9}; Soybean oil {0.15}; Onion, raw {0.9}; Garlic, raw {0.9}</t>
         </is>
       </c>
       <c r="E10" t="inlineStr"/>
@@ -689,7 +705,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Rice, BR-28, boiled* (without salt) {3.0}; Egg, chicken, farmed, boiled* (without salt) {0.33}; Onion, raw {0.17}; Soybean oil {0.15}</t>
+          <t>Rice, BR-28, boiled* (without salt) {3.0}; Egg, chicken, farmed, boiled* (without salt) {0.17}; Onion, raw {0.33}; Soybean oil {0.15}</t>
         </is>
       </c>
       <c r="E12" t="inlineStr"/>
@@ -737,7 +753,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Rice, BR-28, boiled* (without salt) {3.0}; Egg, chicken, farmed, boiled* (without salt) {0.5}; Onion, raw {0.5}; Soybean oil {0.15}; Green gram, split, boiled* (without salt) {0.5}; Gourd, ash, raw {0.5}; Prawn, Giant tiger prawn, raw {0.5}</t>
+          <t>Rice, BR-28, boiled* (without salt) {3.0}; Egg, chicken, farmed, boiled* (without salt) {0.5}; Onion, raw {1.12}; Soybean oil {0.15}; Green gram, split, boiled* (without salt) {1.12}; Gourd, ash, raw {1.12}; Prawn, Giant tiger prawn, raw {1.12}</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -775,7 +791,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Bread, bun/roll {1.0}; UNKNOWN; Water, drinking {2.5}</t>
+          <t>Bread, bun/roll {1.0}; Egg, chicken, farmed, boiled* (without salt) {0.17}; Tomato, red, ripe, boiled* (without salt) {0.11}; Chilli, green, with seeds, raw {0.11}; Onion, raw {0.11}; Turmeric, dried {0.1}; Soybean oil {0.15}; Water, drinking {2.5}</t>
         </is>
       </c>
       <c r="E16" t="inlineStr"/>
@@ -815,7 +831,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Rice, BR-28, boiled* (without salt) {3.0}; Chicken leg, without skin, raw {1.3}; Potato, Diamond, boiled* (without salt) {0.7}; Water, drinking {2.5}</t>
+          <t>Rice, BR-28, boiled* (without salt) {3.0}; Chicken leg, without skin, raw {1.57}; Potato, Diamond, boiled* (without salt) {2.92}; Water, drinking {2.5}</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -841,7 +857,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Chicken leg, without skin, raw {1.3}; Potato, Diamond, boiled* (without salt) {0.7}; Banana, Sagar, ripe, raw {0.5}; Biscuit, sweet* {0.5}; Orange juice, raw (unsweetened) {3.0}</t>
+          <t>Chicken leg, without skin, raw {1.57}; Potato, Diamond, boiled* (without salt) {2.92}; Banana, Sagar, ripe, raw {0.5}; Biscuit, sweet* {0.5}; Orange juice, raw (unsweetened) {3.0}</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -875,7 +891,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Bread, bun/roll {1.0}; UNKNOWN; Chilli, red, dry {0.1}; Soybean oil {0.15}; Water, drinking {5.0}</t>
+          <t>Bread, bun/roll {1.0}; Potato, Diamond, boiled* (without salt) {9.0}; Turmeric, dried {0.1}; Chilli, red, dry {0.1}; Soybean oil {0.15}; Water, drinking {5.0}</t>
         </is>
       </c>
       <c r="E21" t="inlineStr"/>
@@ -911,7 +927,7 @@
       <c r="C23" t="inlineStr"/>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Rice, BR-28, boiled* (without salt) {3.0}; Chicken leg, without skin, raw {4.0}; Water, drinking {2.5}</t>
+          <t>Rice, BR-28, boiled* (without salt) {3.0}; Chicken leg, without skin, raw {9.0}; Water, drinking {2.5}</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -951,7 +967,7 @@
       <c r="C25" t="inlineStr"/>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Rice, BR-28, boiled* (without salt) {3.0}; Chicken leg, without skin, raw {1.95}; Potato, Diamond, boiled* (without salt) {0.53}; Green gram, split, boiled* (without salt) {0.53}; Turmeric, dried {0.1}; Chilli, red, dry {0.1}; UNKNOWN</t>
+          <t>Rice, BR-28, boiled* (without salt) {3.0}; Chicken leg, without skin, raw {1.05}; Potato, Diamond, boiled* (without salt) {0.97}; Green gram, split, boiled* (without salt) {0.97}; Turmeric, dried {0.1}; Chilli, red, dry {0.1}; Salt {0.1}</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -981,7 +997,7 @@
       <c r="C27" t="inlineStr"/>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Bread, bun/roll {1.0}; UNKNOWN; Water, drinking {2.5}</t>
+          <t>Bread, bun/roll {1.0}; Potato, Diamond, boiled* (without salt) {1.5}; Chilli, red, dry {0.1}; Turmeric, dried {0.1}; Onion, raw {1.5}; Soybean oil {0.15}; Mustard oil {0.15}; Water, drinking {2.5}</t>
         </is>
       </c>
       <c r="E27" t="inlineStr"/>
@@ -999,7 +1015,7 @@
       <c r="C28" t="inlineStr"/>
       <c r="D28" t="inlineStr">
         <is>
-          <t>UNKNOWN; Emblic, raw {0.5}; Water, drinking {1.5}</t>
+          <t>UNKNOWN; Emblic, raw {0.5}; Water, drinking {1.25}</t>
         </is>
       </c>
       <c r="E28" t="inlineStr"/>
@@ -1021,7 +1037,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Rice, BR-28, boiled* (without salt) {3.0}; Pangas, without bones, raw {1.3}; Potato, Diamond, boiled* (without salt) {0.17}; Onion, raw {0.17}; Chilli, red, dry {0.1}; Soybean, dried, raw {0.17}; Soybean oil {0.15}; Cauliflower, boiled* (without salt) {0.17}</t>
+          <t>Rice, BR-28, boiled* (without salt) {3.0}; Pangas, without bones, raw {1.57}; Potato, Diamond, boiled* (without salt) {0.73}; Onion, raw {0.73}; Chilli, red, dry {0.1}; Soybean, dried, raw {0.73}; Soybean oil {0.15}; Cauliflower, boiled* (without salt) {0.73}</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -1097,10 +1113,14 @@
       <c r="C33" t="inlineStr"/>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Rice, BR-28, boiled* (without salt) {3.0}; UNKNOWN; Water, drinking {2.5}</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr"/>
+          <t>Rice, BR-28, boiled* (without salt) {3.0}; Pangas, without bones, raw {1.05}; Potato, Diamond, boiled* (without salt) {0.97}; Onion, raw {0.97}; Chilli, red, dry {0.1}; Turmeric, dried {0.1}; Water, drinking {2.5}</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Pangas, without bones, raw</t>
+        </is>
+      </c>
       <c r="F33" t="inlineStr"/>
     </row>
     <row r="34">
@@ -1127,7 +1147,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Bread, bun/roll {1.0}; UNKNOWN; Soybean oil {0.15}; UNKNOWN; Coriander leaves, raw {0.1}; Water, drinking {2.5}</t>
+          <t>Bread, bun/roll {1.0}; Potato, Diamond, boiled* (without salt) {1.5}; Tomato, red, ripe, boiled* (without salt) {1.5}; Soybean oil {0.15}; Chilli, green, with seeds, raw {1.5}; Coriander seed, dry {0.1}; Coriander leaves, raw {0.1}; Water, drinking {2.5}</t>
         </is>
       </c>
       <c r="E35" t="inlineStr"/>
@@ -1149,7 +1169,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Rice, BR-28, boiled* (without salt) {3.0}; Pangas, without bones, raw {0.33}; Amaranth, leaves, red, boiled* (without salt) {0.17}; Coriander leaves, raw {0.1}</t>
+          <t>Rice, BR-28, boiled* (without salt) {3.0}; Pangas, without bones, raw {0.17}; Amaranth, leaves, red, boiled* (without salt) {0.33}; Coriander leaves, raw {0.1}</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -1219,7 +1239,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Rice, BR-28, boiled* (without salt) {3.0}; UNKNOWN; Onion, raw {0.67}; Soybean oil {0.15}; Green gram, split, boiled* (without salt) {0.67}; Turmeric, dried {0.1}; Chilli, red, dry {0.1}; Onion, raw {0.67}; UNKNOWN; Orange juice, raw (unsweetened) {5.0}</t>
+          <t>Rice, BR-28, boiled* (without salt) {3.0}; Potato, Diamond, boiled* (without salt) {0.5}; Chilli, red, dry {0.1}; Onion, raw {0.5}; Soybean oil {0.15}; Green gram, split, boiled* (without salt) {0.5}; Turmeric, dried {0.1}; Chilli, red, dry {0.1}; Onion, raw {0.5}; Salt {0.1}; Orange juice, raw (unsweetened) {5.0}</t>
         </is>
       </c>
       <c r="E40" t="inlineStr"/>
@@ -1259,7 +1279,7 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Rice, BR-28, boiled* (without salt) {3.0}; UNKNOWN; Onion, raw {1.0}; Soybean oil {0.15}; Green gram, split, boiled* (without salt) {1.0}; Turmeric, dried {0.1}; Chilli, red, dry {0.1}; Onion, raw {1.0}; UNKNOWN; Water, drinking {5.0}</t>
+          <t>Rice, BR-28, boiled* (without salt) {3.0}; Potato, Diamond, boiled* (without salt) {1.38}; Chilli, red, dry {0.1}; Onion, raw {1.38}; Soybean oil {0.15}; Green gram, split, boiled* (without salt) {1.38}; Turmeric, dried {0.1}; Chilli, red, dry {0.1}; Onion, raw {1.38}; Salt {0.1}; Water, drinking {5.0}</t>
         </is>
       </c>
       <c r="E42" t="inlineStr"/>
@@ -1329,7 +1349,7 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Bread, bun/roll {1.0}; UNKNOWN; Onion, raw {2.0}; Soybean oil {0.15}; Water, drinking {5.0}</t>
+          <t>Bread, bun/roll {1.0}; Potato, Diamond, boiled* (without salt) {2.25}; Onion, raw {2.25}; Soybean oil {0.15}; Water, drinking {5.0}</t>
         </is>
       </c>
       <c r="E46" t="inlineStr"/>
@@ -1369,10 +1389,14 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Rice, BR-28, boiled* (without salt) {3.0}; UNKNOWN; Tomato, red, ripe, boiled* (without salt) {1.33}; Onion, raw {1.33}; Soybean oil {0.15}; UNKNOWN; Onion, raw {1.33}; Soybean oil {0.15}; UNKNOWN; Water, drinking {2.5}</t>
-        </is>
-      </c>
-      <c r="E48" t="inlineStr"/>
+          <t>Rice, BR-28, boiled* (without salt) {3.0}; Pangas, without bones, raw {3.15}; Tomato, red, ripe, boiled* (without salt) {1.17}; Onion, raw {1.17}; Soybean oil {0.15}; Potato, Diamond, boiled* (without salt) {1.17}; Onion, raw {1.17}; Soybean oil {0.15}; Pumpkin leaves, raw {1.17}; Water, drinking {2.5}</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Pangas, without bones, raw</t>
+        </is>
+      </c>
       <c r="F48" t="inlineStr"/>
     </row>
     <row r="49">
@@ -1387,7 +1411,7 @@
       <c r="C49" t="inlineStr"/>
       <c r="D49" t="inlineStr">
         <is>
-          <t>UNKNOWN; UNKNOWN; UNKNOWN; Biscuit, sweet* {0.75}</t>
+          <t>Potato, Diamond, boiled* (without salt) {0.43}; Carrot, boiled* (without salt) {0.43}; Onion, raw {0.43}; Soybean oil {0.15}; Chilli, green, with seeds, raw {0.43}; Potato, Diamond, boiled* (without salt) {0.43}; Onion, raw {0.43}; Chilli, green, with seeds, raw {0.43}; Soybean oil {0.15}; UNKNOWN; Biscuit, sweet* {0.75}</t>
         </is>
       </c>
       <c r="E49" t="inlineStr"/>
@@ -1409,10 +1433,14 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>UNKNOWN; Onion, raw {0.17}; Chilli, red, dry {0.1}; Coriander leaves, raw {0.1}; UNKNOWN; Soybean oil {0.15}; Onion, raw {0.17}; Tomato, red, ripe, boiled* (without salt) {0.17}; Green gram, split, boiled* (without salt) {0.17}; Onion, raw {0.17}; Coriander leaves, raw {0.1}; Garlic, raw {0.17}; Soybean oil {0.15}; Rice, BR-28, boiled* (without salt) {1.5}; Water, drinking {1.5}</t>
-        </is>
-      </c>
-      <c r="E50" t="inlineStr"/>
+          <t>Egg, chicken, farmed, boiled* (without salt) {0.17}; Onion, raw {0.11}; Chilli, red, dry {0.1}; Coriander leaves, raw {0.1}; Pangas, without bones, raw {0.17}; Soybean oil {0.15}; Onion, raw {0.11}; Tomato, red, ripe, boiled* (without salt) {0.11}; Green gram, split, boiled* (without salt) {0.11}; Onion, raw {0.11}; Coriander leaves, raw {0.1}; Garlic, raw {0.11}; Soybean oil {0.15}; Rice, BR-28, boiled* (without salt) {1.5}; Water, drinking {1.25}</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Pangas, without bones, raw</t>
+        </is>
+      </c>
       <c r="F50" t="inlineStr"/>
     </row>
     <row r="51">
@@ -1439,7 +1467,7 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Bread, bun/roll {1.0}; UNKNOWN; Water, drinking {2.5}</t>
+          <t>Bread, bun/roll {1.0}; Egg, chicken, farmed, boiled* (without salt) {1.57}; Tomato, red, ripe, boiled* (without salt) {0.97}; Chilli, green, with seeds, raw {0.97}; Onion, raw {0.97}; Turmeric, dried {0.1}; Soybean oil {0.15}; Water, drinking {2.5}</t>
         </is>
       </c>
       <c r="E52" t="inlineStr"/>
@@ -1461,10 +1489,14 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Rice, BR-28, boiled* (without salt) {3.0}; UNKNOWN; Onion, raw {1.5}; Chilli, red, dry {0.1}; Soybean oil {0.15}; Cauliflower, boiled* (without salt) {1.5}; UNKNOWN; Water, drinking {5.0}</t>
-        </is>
-      </c>
-      <c r="E53" t="inlineStr"/>
+          <t>Rice, BR-28, boiled* (without salt) {3.0}; Pangas, without bones, raw {1.05}; Potato, Diamond, boiled* (without salt) {0.65}; Onion, raw {0.65}; Chilli, red, dry {0.1}; Soybean oil {0.15}; Cauliflower, boiled* (without salt) {0.65}; UNKNOWN; Water, drinking {5.0}</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Pangas, without bones, raw</t>
+        </is>
+      </c>
       <c r="F53" t="inlineStr"/>
     </row>
     <row r="54">
@@ -1501,7 +1533,7 @@
       <c r="C55" t="inlineStr"/>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Biscuit, sweet* {1.5}</t>
+          <t>Biscuit, sweet* {4.5}</t>
         </is>
       </c>
       <c r="E55" t="inlineStr"/>
@@ -1519,10 +1551,14 @@
       <c r="C56" t="inlineStr"/>
       <c r="D56" t="inlineStr">
         <is>
-          <t>UNKNOWN; Radish, boiled* (without salt) {1.5}; UNKNOWN; Cucumber, peeled, raw {1.5}; Soybean oil {0.15}; UNKNOWN</t>
-        </is>
-      </c>
-      <c r="E56" t="inlineStr"/>
+          <t>Pangas, without bones, raw {1.05}; Tomato, red, ripe, boiled* (without salt) {0.65}; Radish, boiled* (without salt) {0.65}; UNKNOWN; Cucumber, peeled, raw {0.65}; Soybean oil {0.15}; UNKNOWN</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Pangas, without bones, raw</t>
+        </is>
+      </c>
       <c r="F56" t="inlineStr"/>
     </row>
     <row r="57">
@@ -1567,10 +1603,14 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Rice, BR-28, boiled* (without salt) {3.0}; UNKNOWN; Turmeric, dried {0.1}; Chilli, green, with seeds, raw {1.5}; Soybean oil {0.15}; Green gram, split, boiled* (without salt) {1.5}; Chilli, red, dry {0.1}; Turmeric, dried {0.1}</t>
-        </is>
-      </c>
-      <c r="E59" t="inlineStr"/>
+          <t>Rice, BR-28, boiled* (without salt) {3.0}; Pangas, without bones, raw {1.05}; Potato, Diamond, boiled* (without salt) {0.65}; Turmeric, dried {0.1}; Chilli, green, with seeds, raw {0.65}; Soybean oil {0.15}; Green gram, split, boiled* (without salt) {0.65}; Chilli, red, dry {0.1}; Turmeric, dried {0.1}</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>Pangas, without bones, raw</t>
+        </is>
+      </c>
       <c r="F59" t="inlineStr"/>
     </row>
     <row r="60">
@@ -1589,7 +1629,7 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>UNKNOWN; UNKNOWN; Jaggery, sugarcane, solid {1.5}; Payesh* {1.5}</t>
+          <t>Milk, cow, whole fat (pasteurized, UTH) {0.75}; Rice, BR-28, boiled* (without salt) {0.75}; Jaggery, sugarcane, solid {0.75}; Payesh* {0.75}</t>
         </is>
       </c>
       <c r="E60" t="inlineStr"/>
@@ -1611,10 +1651,14 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Rice, BR-28, boiled* (without salt) {3.0}; UNKNOWN; Soybean oil {0.15}; Green gram, split, boiled* (without salt) {3.0}; Chilli, red, dry {0.1}; Turmeric, dried {0.1}; UNKNOWN</t>
-        </is>
-      </c>
-      <c r="E61" t="inlineStr"/>
+          <t>Rice, BR-28, boiled* (without salt) {3.0}; Pangas, without bones, raw {1.05}; Potato, Diamond, boiled* (without salt) {0.33}; Soybean oil {0.15}; Green gram, split, boiled* (without salt) {0.33}; Chilli, red, dry {0.1}; Turmeric, dried {0.1}; Brinjal, purple, long, boiled* (without salt) {0.33}; Potato, Diamond, boiled* (without salt) {0.33}; Radish, boiled* (without salt) {0.33}; Spinach, boiled* (without salt) {0.33}</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>Pangas, without bones, raw</t>
+        </is>
+      </c>
       <c r="F61" t="inlineStr"/>
     </row>
     <row r="62">
@@ -1641,7 +1685,7 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Rice, BR-28, boiled* (without salt) {3.0}; Spinach, boiled* (without salt) {2.0}; Soybean oil {0.15}; Water, drinking {2.5}</t>
+          <t>Rice, BR-28, boiled* (without salt) {3.0}; Spinach, boiled* (without salt) {4.5}; Soybean oil {0.15}; Water, drinking {2.5}</t>
         </is>
       </c>
       <c r="E63" t="inlineStr"/>
@@ -1663,10 +1707,14 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Rice, BR-28, boiled* (without salt) {3.0}; UNKNOWN; Water, drinking {2.5}</t>
-        </is>
-      </c>
-      <c r="E64" t="inlineStr"/>
+          <t>Rice, BR-28, boiled* (without salt) {3.0}; Chicken leg, without skin, raw {1.57}; Onion, raw {1.46}; Garlic, raw {1.46}; Ginger root, raw {0.1}; Chilli, red, dry {0.1}; Water, drinking {2.5}</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>Chicken leg, without skin, raw</t>
+        </is>
+      </c>
       <c r="F64" t="inlineStr"/>
     </row>
     <row r="65">
@@ -1681,7 +1729,7 @@
       <c r="C65" t="inlineStr"/>
       <c r="D65" t="inlineStr">
         <is>
-          <t>UNKNOWN; Orange juice, raw (unsweetened) {1.5}</t>
+          <t>UNKNOWN; Orange juice, raw (unsweetened) {1.25}</t>
         </is>
       </c>
       <c r="E65" t="inlineStr"/>
@@ -1703,7 +1751,7 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Hog plum, raw {3.0}; UNKNOWN; Chilli, red, dry {0.1}</t>
+          <t>Hog plum, raw {3.0}; Salt {0.1}; Chilli, red, dry {0.1}</t>
         </is>
       </c>
       <c r="E66" t="inlineStr"/>
@@ -1725,7 +1773,7 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Rice, puffed, salted {1.0}; Tomato, red, ripe, boiled* (without salt) {1.0}; Chilli, red, dry {0.1}; Coriander leaves, raw {0.1}; Water, drinking {5.0}</t>
+          <t>Rice, puffed, salted {2.25}; Tomato, red, ripe, boiled* (without salt) {2.25}; Chilli, red, dry {0.1}; Coriander leaves, raw {0.1}; Water, drinking {5.0}</t>
         </is>
       </c>
       <c r="E67" t="inlineStr"/>

</xml_diff>